<commit_message>
delete not useful module
</commit_message>
<xml_diff>
--- a/plan/游戏学院1809A开发班级实训一项目开发计划.xlsx
+++ b/plan/游戏学院1809A开发班级实训一项目开发计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9372" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="第一周" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="101">
   <si>
     <t>游戏学院1809A开发班实训一周开发计划</t>
   </si>
@@ -473,16 +473,25 @@
 腾讯云直播页面（1天）</t>
   </si>
   <si>
+    <t>分享QQ用户，推送消息，云直播功能</t>
+  </si>
+  <si>
     <t>第三方登录（1天）
 电话,地址(1天)
 代码优化（1天）
 网络状态的判断（1天）</t>
   </si>
   <si>
+    <t>消息管理，推送消息到消息页面，代码优化，地图地址</t>
+  </si>
+  <si>
     <t>退出登录和打电话（1）
 友盟推送（1）
 退出登录（1）
 环信（1）</t>
+  </si>
+  <si>
+    <t>传输地址,支付方式，网络状态</t>
   </si>
   <si>
     <t>电话和地址（1）
@@ -506,17 +515,11 @@
 地图地址（1天）</t>
   </si>
   <si>
-    <t>消息管理，推送消息到消息页面，代码优化，地图地址</t>
-  </si>
-  <si>
     <t xml:space="preserve">电话,地址(1天)
 支付方式（1天）
 代码优化（1天）
 网络状态的判断（1天）
 </t>
-  </si>
-  <si>
-    <t>传输地址,支付方式，网络状态</t>
   </si>
 </sst>
 </file>
@@ -525,8 +528,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="33">
@@ -623,15 +626,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -653,6 +648,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -660,29 +677,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -697,7 +693,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -711,8 +730,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -726,16 +746,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -743,24 +755,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -771,7 +774,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -822,187 +825,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1081,21 +1072,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1111,22 +1087,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1134,8 +1105,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1157,24 +1128,44 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1186,10 +1177,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1198,133 +1189,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1811,19 +1802,19 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="21.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.8796296296296" style="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.8796296296296" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.375" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="1"/>
+    <col min="6" max="6" width="31.3796296296296" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6296296296296" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.87962962962963" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25.5" spans="1:7">
+    <row r="1" ht="25.8" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1834,7 +1825,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" ht="18.75" spans="1:7">
+    <row r="2" ht="17.4" spans="1:7">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2046,7 +2037,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" ht="156.75" spans="1:5">
+    <row r="15" ht="171.6" spans="1:5">
       <c r="A15" s="8" t="s">
         <v>47</v>
       </c>
@@ -2063,7 +2054,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" ht="114" spans="1:5">
+    <row r="16" ht="124.8" spans="1:5">
       <c r="A16" s="8"/>
       <c r="B16" s="9" t="s">
         <v>52</v>
@@ -2093,21 +2084,21 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" ht="14.25" hidden="1" spans="1:5">
+    <row r="18" ht="15.6" hidden="1" spans="1:5">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="15"/>
       <c r="D18" s="11"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" ht="14.25" hidden="1" spans="1:5">
+    <row r="19" ht="15.6" hidden="1" spans="1:5">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="15"/>
       <c r="D19" s="11"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" ht="14.25" hidden="1" spans="1:5">
+    <row r="20" ht="15.6" hidden="1" spans="1:5">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="15"/>
@@ -2144,23 +2135,23 @@
   <sheetPr/>
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="21.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.8796296296296" style="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.8796296296296" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.375" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="1"/>
+    <col min="6" max="6" width="31.3796296296296" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6296296296296" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.87962962962963" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25.5" spans="1:7">
+    <row r="1" ht="25.8" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -2171,7 +2162,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" ht="18.75" spans="1:7">
+    <row r="2" ht="17.4" spans="1:7">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2682,23 +2673,23 @@
   <sheetPr/>
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="21.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.8796296296296" style="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.8796296296296" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.375" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="1"/>
+    <col min="6" max="6" width="31.3796296296296" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6296296296296" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.87962962962963" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25.5" spans="1:7">
+    <row r="1" ht="25.8" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>89</v>
       </c>
@@ -2709,7 +2700,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" ht="18.75" spans="1:7">
+    <row r="2" ht="17.4" spans="1:7">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2817,7 +2808,9 @@
       <c r="C8" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="20" t="s">
+        <v>91</v>
+      </c>
       <c r="E8" s="21"/>
       <c r="F8" s="17"/>
       <c r="G8" s="13"/>
@@ -2846,9 +2839,11 @@
         <v>31</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="20"/>
+        <v>92</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>93</v>
+      </c>
       <c r="E11" s="31"/>
       <c r="F11" s="3"/>
       <c r="G11" s="13"/>
@@ -2870,9 +2865,11 @@
         <v>37</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="20"/>
+        <v>94</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>95</v>
+      </c>
       <c r="E13" s="20"/>
       <c r="F13" s="17"/>
       <c r="G13" s="13"/>
@@ -2892,9 +2889,11 @@
         <v>35</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="20"/>
+        <v>96</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>95</v>
+      </c>
       <c r="E15" s="20"/>
       <c r="F15" s="17"/>
       <c r="G15" s="13"/>
@@ -2975,10 +2974,10 @@
         <v>52</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E22" s="20"/>
     </row>
@@ -3051,10 +3050,10 @@
         <v>56</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E32" s="31"/>
     </row>
@@ -3106,10 +3105,10 @@
         <v>48</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E39" s="31"/>
     </row>
@@ -3216,7 +3215,7 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>